<commit_message>
i added new files
</commit_message>
<xml_diff>
--- a/DSA Sheet by Arsh (45 Days Plan).xlsx
+++ b/DSA Sheet by Arsh (45 Days Plan).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agarw\OneDrive\Desktop\Dsa\Arsh280\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5950AD-862A-405B-9DC6-05AEA91C5F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB9EA44-EC02-4611-B4D5-262049A04906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="385">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1708,8 +1708,8 @@
   </sheetPr>
   <dimension ref="A1:I340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C203" sqref="C203"/>
+    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="C306" sqref="C306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5216,22 +5216,28 @@
     </row>
     <row r="304" spans="1:8" ht="12.75">
       <c r="A304" s="5" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="B304" s="9" t="s">
         <v>294</v>
       </c>
+      <c r="C304" t="s">
+        <v>329</v>
+      </c>
       <c r="F304" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="305" spans="1:8" ht="12.75">
-      <c r="A305" s="5" t="s">
-        <v>244</v>
+      <c r="A305" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B305" s="15" t="s">
         <v>295</v>
       </c>
+      <c r="C305" t="s">
+        <v>329</v>
+      </c>
       <c r="D305" s="5" t="s">
         <v>11</v>
       </c>
@@ -5240,24 +5246,27 @@
       </c>
     </row>
     <row r="306" spans="1:8" ht="12.75">
-      <c r="A306" s="5" t="s">
-        <v>244</v>
+      <c r="A306" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B306" s="9" t="s">
         <v>296</v>
       </c>
+      <c r="C306" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="307" spans="1:8" ht="12.75">
-      <c r="A307" s="5" t="s">
-        <v>244</v>
+      <c r="A307" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B307" s="9" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="308" spans="1:8" ht="12.75">
-      <c r="A308" s="5" t="s">
-        <v>244</v>
+      <c r="A308" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B308" s="9" t="s">
         <v>298</v>
@@ -5267,8 +5276,8 @@
       </c>
     </row>
     <row r="309" spans="1:8" ht="12.75">
-      <c r="A309" s="5" t="s">
-        <v>244</v>
+      <c r="A309" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B309" s="9" t="s">
         <v>299</v>
@@ -5278,8 +5287,8 @@
       </c>
     </row>
     <row r="310" spans="1:8" ht="12.75">
-      <c r="A310" s="5" t="s">
-        <v>244</v>
+      <c r="A310" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B310" s="7" t="s">
         <v>300</v>
@@ -5289,8 +5298,8 @@
       </c>
     </row>
     <row r="311" spans="1:8" ht="12.75">
-      <c r="A311" s="5" t="s">
-        <v>244</v>
+      <c r="A311" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B311" s="9" t="s">
         <v>301</v>
@@ -5300,8 +5309,8 @@
       </c>
     </row>
     <row r="312" spans="1:8" ht="12.75">
-      <c r="A312" s="5" t="s">
-        <v>244</v>
+      <c r="A312" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B312" s="9" t="s">
         <v>302</v>
@@ -5314,8 +5323,8 @@
       </c>
     </row>
     <row r="313" spans="1:8" ht="12.75">
-      <c r="A313" s="5" t="s">
-        <v>244</v>
+      <c r="A313" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B313" s="7" t="s">
         <v>303</v>

</xml_diff>